<commit_message>
SEFERLER arayüzü revize edildi
</commit_message>
<xml_diff>
--- a/DEV_NOTES/isleyis_semalari.xlsx
+++ b/DEV_NOTES/isleyis_semalari.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayhan\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayhan\SATTUP\DEV_NOTES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5500E5AF-7FEA-4D04-A746-203DAA247E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA5E67F-E14D-4D20-A01C-3B478E7D957C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sözleşmeler" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="182">
   <si>
     <t>QLineEdit</t>
   </si>
@@ -287,18 +287,6 @@
     <t>table_rotalar</t>
   </si>
   <si>
-    <t>btn_ekle</t>
-  </si>
-  <si>
-    <t>btn_cikar</t>
-  </si>
-  <si>
-    <t>EKLE</t>
-  </si>
-  <si>
-    <t>ÇIKAR</t>
-  </si>
-  <si>
     <t>İNDİ BİNDİ NOKTA EKLEME</t>
   </si>
   <si>
@@ -428,9 +416,6 @@
     <t>QTabWidget</t>
   </si>
   <si>
-    <t>QStackedWidget</t>
-  </si>
-  <si>
     <t>QTextEdit</t>
   </si>
   <si>
@@ -449,39 +434,12 @@
     <t>cmb_service_type</t>
   </si>
   <si>
-    <t>Tip</t>
-  </si>
-  <si>
     <t>txt_kalem_sec</t>
   </si>
   <si>
     <t>placeholder</t>
   </si>
   <si>
-    <t>lbl_hareket</t>
-  </si>
-  <si>
-    <t>time_g1</t>
-  </si>
-  <si>
-    <t>GİRİŞ</t>
-  </si>
-  <si>
-    <t>time_c1</t>
-  </si>
-  <si>
-    <t>time_g2</t>
-  </si>
-  <si>
-    <t>time_g3</t>
-  </si>
-  <si>
-    <t>time_c2</t>
-  </si>
-  <si>
-    <t>ÇIKIŞ</t>
-  </si>
-  <si>
     <t>cmb_arac_sec</t>
   </si>
   <si>
@@ -500,75 +458,9 @@
     <t>ARAÇ VE SÜRÜ..</t>
   </si>
   <si>
-    <t>btn_yenile</t>
-  </si>
-  <si>
-    <t>tbl_grid</t>
-  </si>
-  <si>
-    <t>YENİLE</t>
-  </si>
-  <si>
-    <t>kullanıcı  cmb_service_type ile veri seçtiğinde</t>
-  </si>
-  <si>
-    <t xml:space="preserve">list_kalemlerde satır seçince başlangıçta enabled false olan bu time inputlar enablde true olur ve kullanıcı 1.Vardiya giriş saatini yazacak, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">list_kalemlerde satır seçince başlangıçta enabled false olan bu time inputlar enablde true olur ve kullanıcı 1.Vardiya çıkış saatini yazacak, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">list_kalemlerde satır seçince başlangıçta enabled false olan bu time inputlar enablde true olur ve kullanıcı 2.Vardiya giriş saatini yazacak, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">list_kalemlerde satır seçince başlangıçta enabled false olan bu time inputlar enablde true olur ve kullanıcı 2.Vardiya çıkış saatini yazacak, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">list_kalemlerde satır seçince başlangıçta enabled false olan bu time inputlar enablde true olur ve kullanıcı 3.Vardiya giriş saatini yazacak, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">list_kalemlerde satır seçince başlangıçta enabled false olan bu time inputlar enablde true olur ve kullanıcı 3.Vardiya çıkış saatini yazacak, </t>
-  </si>
-  <si>
-    <t>list_kalemlerde satır seçilir (satır seçili kalır), sonra time_g1 ile time_c1 seçilir. (bu nesnelerde seçili kalır), Sonra cmb_arac_sec ile cmb_surucu_sec den veriler(araç ve Şoför seçilir) bütün seçilen yerler (list_kalemler, time_g1, time_c1, cmb_arac|sec ile cmb_surucu_sec deki bilgiler list_kalemlerdeki rotanın 1. seferi olur. list_kalemlerde sırayla yazılı rotaların sefer olarak planlanmamış veya plnalı birden fazla sefer olabilir. Yani hiç bir zaman if Rota= 1 sefer anlaşılmasın.. Örneğin: Planlanmış olan bir rotada 5 ayrı araç ve sürücü ile 3 farklı sefer de yapılabilir. ayrıca aynı araç ve sürücü aynı gün 3 vardiya hatta birde mesai sefer olma üzere 4 vardiya(Gidiş bir hareket, geliş de bir hareket olarak sayıldığında bir şoför aynı günde 4 çift servis (8 hareket yapabilir.)</t>
-  </si>
-  <si>
-    <t>kullanıcı  cmb_service_type ile veri seçtiğinde bu üç inputun karşılığı olan route_params. route_name kolonu  &amp; indibindi_dialog.ui-txt_indibindi &amp; distance_km şeklinde load olur</t>
-  </si>
-  <si>
-    <t>list_kalemler den başlayarak araç ve sürücü ataması yapıldıktan sonra kullanıcı tarafından tetiklenerek tüm seçilen alanlar tbl.grid load edilir.</t>
-  </si>
-  <si>
-    <t>tüm sayfanın (formun) yenilenmesini tetikler</t>
-  </si>
-  <si>
-    <t>kullanıcı tarafından girilmiş ama henüz btn_ekle tetiklenmediyse tüm inputları boşaltır.</t>
-  </si>
-  <si>
-    <t>tbl.gride load edilmiş en son durumu db ye kaydeder.</t>
-  </si>
-  <si>
-    <t>btn_kaydet ile db ye kaydedilen bilgileri siler (admin kullanıcı yetkisi)</t>
-  </si>
-  <si>
-    <t>form açılışında önceden yapılıp db ye kaydedilmiş "sefer" bilgileri load edilir.</t>
-  </si>
-  <si>
-    <t>Label otomatik (dinamik) dolacak. = "HAREKET TÜRÜ: &amp; hat_dialog.ui-table_kalemler.column(1) &amp; contracts.ui-cmb_vardiya value &amp; "VARDİYA"</t>
-  </si>
-  <si>
-    <t>time_c3</t>
-  </si>
-  <si>
-    <t>tbl.grid'de seçili satırdaki araç ve sürücüyü çıkarır ve yensinin eklenmesi için cmb_arac_sec focus olur.</t>
-  </si>
-  <si>
     <t>s.no</t>
   </si>
   <si>
-    <t>QTimeEdit nesneleri form açılışında özellikleri enabled false olacak. List_kalemler de seçilen satır "seçili" kalacak. "seçili" kalan satıra ait olacak olan sırayla dolacak olan inputlarda  btn_ekle tetikleninceye kadar tüm bilgiler  list_kalemlerde "seçili"olan satır bigilerine ait olacak.  yukarıdaki tabloda 8 - 22 arasındaki tüm nesenler enablde false olacak. 7.maddeden sonra 8-13 arası nesneler (QTimeEdit) enabled=true olacak. Time nesneleri bitince 14-15-16 enbaled true, 16.ncıdan sonra da diğerleri enabled true olacak şekilde bir yapının olabilirliğine göre yapılsın..</t>
-  </si>
-  <si>
     <t>cmb_vardiya</t>
   </si>
   <si>
@@ -588,6 +480,99 @@
   </si>
   <si>
     <t>kullanıcı, "-,1,2,3,4" rakamlarından uygun olanı seçecek.</t>
+  </si>
+  <si>
+    <t>list_kalemler de bulunan verileri filtreler</t>
+  </si>
+  <si>
+    <t>table_sefer</t>
+  </si>
+  <si>
+    <t>trips_dialog_ui de iş kalemi için girilen alt bilgilerin (sefer tipi, giriş çıkış saatleri araç ve sürücü atama) kaydedildikten sonra bu tabloya sırayla aktarılır.</t>
+  </si>
+  <si>
+    <t>btn_delete_all</t>
+  </si>
+  <si>
+    <t>TÜM SEFERLERİ SİL</t>
+  </si>
+  <si>
+    <t>trips_dialog.ui de kaydedilip table_sefer de aktarılan bilgileri sefer olarak kaydeder</t>
+  </si>
+  <si>
+    <t>table_sefer de seçili satırın silinmesini sağlar</t>
+  </si>
+  <si>
+    <t>table_sefer de bulunan tüm seferli siler</t>
+  </si>
+  <si>
+    <t>SEFER TİPİ VE ARAÇ SÜRÜCÜ ATAMA FORMU</t>
+  </si>
+  <si>
+    <t>UI adı: trips_dialog.ui</t>
+  </si>
+  <si>
+    <t>chk_vardiya1</t>
+  </si>
+  <si>
+    <t>chk_vardiya2</t>
+  </si>
+  <si>
+    <t>chk_vardiya3</t>
+  </si>
+  <si>
+    <t>chk_mesai1</t>
+  </si>
+  <si>
+    <t>chk_mesai2</t>
+  </si>
+  <si>
+    <t>chk_ek_sefer</t>
+  </si>
+  <si>
+    <t>VARDİYA-1 SEFER</t>
+  </si>
+  <si>
+    <t>MESAİ-1 SEFER</t>
+  </si>
+  <si>
+    <t>EK / ÖZEL SEFER</t>
+  </si>
+  <si>
+    <t>VARDİYA-2 SEFER</t>
+  </si>
+  <si>
+    <t>VARDİYA-3 SEFER</t>
+  </si>
+  <si>
+    <t>MESAİ-2 SEFER</t>
+  </si>
+  <si>
+    <t>ilgili iş kaleminin vardiyalı seferleri olduğunda vardiya sayısına göre seçim yapılarak her yapılan seçim ile ilgili seçime ait giriş ve çıkış saatlerinin inputları enabled olur. Örnek: x işkaleminin 3 vardiya ve 1 mesai seferi olduğunu varsayalım. = chk_vardiya1 seçilir, cmb_vardiya1_g ile cmb_vardiya1_c inputları veri girilebilmesi için enabled duruma geçer, veriler girildikten sonra  seferi gerçekleştirecek araç ve sürücü ataması için ilgili alanlar (cmb_arac_sec ile cmb_surucu_sec) doldurulur ve btn_atama tetiklenerek  ilgili işkaleminin vardıya1-sefer tibi giriş-çıkış saatleri ile araç ve sürücüsü atanmış bir sefer planlanmış olur. seferlerin table_sefere aktarılması için btn_kaydet tetiklenir. (işkalemine at tüm seferlerin aynı araç ve sürücü ile seferi planlanmak istendiğinde toplu halde de yapılacak. hangi QCheckBox u seçili tüm sefer tipleri için tek bir araç ve sürücü seçilip kaydedilebilir.</t>
+  </si>
+  <si>
+    <t>Dialog formu üzirnde 6 adet QCheckBox bulunmaktadır. Checkboxu "onay"lı olarak seçili tüm sefer tiplerine</t>
+  </si>
+  <si>
+    <t>dialog formunun tüm nesnelerin temizler. (ilk açılışa gelir)</t>
+  </si>
+  <si>
+    <t>planlanmış seferin table_sefere aktarılmasını sağlar</t>
+  </si>
+  <si>
+    <t>cmb_arac_sec ile cmb_surucu_sec hariç tüm QComboBox nesneleri formun açılışında özellikleri enabled false olacak. Seçimlere göre enabled_tru olacak. Bu kısmı Qt Designer Signal/Slot ile halledildi. Koda gerek yok Bilgi amaçlı yazıldı) List_kalemler de seçilen satır "seçili" kalacak. "seçili" kalan satıra ait bilgileri girmek üzere trips_dialog.ui açılsın demiştik. Toplu atama için trips_dialog.ui de birden fazla sefer tipi seçilmesi ile araç ve sürücü ataması tek seferde planlanabilsin. trips_dialog.ui formundan çıkılmadığı sürece seçilen araç ve sürücü default olarak kalsın.  Kullanıcının list_kalemlerdeki satırın sefer planlaması yapılıp yapılmadığını anlayabilmesi için list_kalemlerde her satırın yanına bir onay sembolü ekekleyelim. seçili satırın planlaması yapılmış ise onaylı henüz planlanmamış ise onaysız görülsün.  daha önce sefer planlaması yapılmış satırın seçimesi durumunda uyarı vererek trips_dialog.ui formu güncelleme modu tarzında açılsın (Kaydet butonu texti "GÜNCELLE" olsun.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kullanıcı  cmb_service_type ile veri seçtiğinde İş Kalemi + Hareket Türü (+ onay kutusu=notlarda yazılı) load olur. list_kalemler de satır seçildiğinde seçili işkalemi için alt bilgilerin girilmesi için trips_dialog.ui açılır. </t>
+  </si>
+  <si>
+    <t>kullanıcı tarafından seçilecek. İTEMS =&gt;Müşteri olarak kaydedilenler.</t>
+  </si>
+  <si>
+    <t>kullanıcı tarafından seçilecek. İTEMS =&gt; seçilen müşteriye ait kaydedilen sözleşmeler</t>
+  </si>
+  <si>
+    <t>kullanıcı tarafından seçilecek. İTEMS =&gt; ÖĞRENCİ TAŞIMA/PERSONEL TAŞIMA/ARAÇ KİRALAMA/DİĞER</t>
   </si>
 </sst>
 </file>
@@ -641,7 +626,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -725,11 +710,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -772,6 +768,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -784,27 +798,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -814,29 +810,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1120,7 +1113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -1137,12 +1130,12 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1158,10 +1151,10 @@
       <c r="D5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="F5" s="17"/>
+      <c r="E5" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5" s="23"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
@@ -1170,13 +1163,13 @@
       <c r="B6" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="21"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
       <c r="E6" s="14" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1190,7 +1183,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>76</v>
@@ -1210,7 +1203,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -1232,7 +1225,7 @@
         <v>76</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1252,7 +1245,7 @@
         <v>76</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1272,7 +1265,7 @@
         <v>76</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1292,7 +1285,7 @@
         <v>76</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1312,7 +1305,7 @@
         <v>76</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1332,7 +1325,7 @@
         <v>76</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1345,14 +1338,14 @@
       <c r="C15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>127</v>
+      <c r="F15" s="24" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1365,38 +1358,38 @@
       <c r="C16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>180</v>
+        <v>144</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>183</v>
+        <v>147</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>186</v>
+        <v>150</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="34" t="s">
-        <v>181</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="D18" s="35" t="s">
-        <v>186</v>
+      <c r="B18" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -1406,32 +1399,32 @@
         <v>2</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>182</v>
+        <v>146</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>185</v>
+        <v>149</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>186</v>
+        <v>150</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
     </row>
-    <row r="20" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="34" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
@@ -1449,21 +1442,21 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="34" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
@@ -1481,19 +1474,19 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="34" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="35" t="s">
+      <c r="C24" s="7"/>
+      <c r="D24" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
@@ -1526,8 +1519,8 @@
       <c r="B30" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="21"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
@@ -1580,7 +1573,7 @@
         <v>35</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1598,29 +1591,29 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="18" t="s">
         <v>58</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C37" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="D37" s="24"/>
+      <c r="D37" s="19"/>
     </row>
     <row r="38" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="23"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="D38" s="26"/>
+      <c r="C38" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="21"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="23"/>
+      <c r="A39" s="18"/>
       <c r="B39" s="7" t="s">
         <v>67</v>
       </c>
@@ -1630,7 +1623,7 @@
       <c r="D39" s="7"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="23"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="7" t="s">
         <v>10</v>
       </c>
@@ -1640,7 +1633,7 @@
       <c r="D40" s="7"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="23"/>
+      <c r="A41" s="18"/>
       <c r="B41" s="7" t="s">
         <v>11</v>
       </c>
@@ -1650,7 +1643,7 @@
       <c r="D41" s="7"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="23"/>
+      <c r="A42" s="18"/>
       <c r="B42" s="7" t="s">
         <v>12</v>
       </c>
@@ -1660,7 +1653,7 @@
       <c r="D42" s="7"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="23"/>
+      <c r="A43" s="18"/>
       <c r="B43" s="7" t="s">
         <v>40</v>
       </c>
@@ -1670,7 +1663,7 @@
       <c r="D43" s="7"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="23"/>
+      <c r="A44" s="18"/>
       <c r="B44" s="7" t="s">
         <v>49</v>
       </c>
@@ -1680,38 +1673,38 @@
       <c r="D44" s="7"/>
     </row>
     <row r="45" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="23"/>
+      <c r="A45" s="18"/>
       <c r="B45" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C45" s="25" t="s">
+      <c r="C45" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="D45" s="26"/>
+      <c r="D45" s="21"/>
     </row>
     <row r="46" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="23"/>
+      <c r="A46" s="18"/>
       <c r="B46" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="25" t="s">
+      <c r="C46" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="D46" s="26"/>
+      <c r="D46" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="D15:D16"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="A37:A46"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="D15:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1806,7 +1799,7 @@
         <v>84</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1818,7 +1811,7 @@
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1826,13 +1819,13 @@
         <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1846,18 +1839,18 @@
         <v>34</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1887,30 +1880,30 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1918,13 +1911,13 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>109</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1944,7 +1937,7 @@
         <v>34</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1958,7 +1951,7 @@
         <v>35</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1990,7 +1983,7 @@
         <v>81</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D28" s="1"/>
     </row>
@@ -2000,7 +1993,7 @@
         <v>83</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D29" s="1"/>
     </row>
@@ -2020,7 +2013,7 @@
         <v>85</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D31" s="1"/>
     </row>
@@ -2036,10 +2029,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2056,12 +2049,12 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="S1" s="9" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="S2" s="9" t="s">
         <v>2</v>
@@ -2069,7 +2062,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="S3" s="9" t="s">
         <v>16</v>
@@ -2077,12 +2070,12 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="S4" s="9" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>3</v>
@@ -2097,7 +2090,7 @@
         <v>28</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
@@ -2110,10 +2103,10 @@
       <c r="C6" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="32"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="31"/>
       <c r="S6" s="9" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
@@ -2130,7 +2123,7 @@
         <v>77</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>60</v>
+        <v>179</v>
       </c>
       <c r="S7" s="9" t="s">
         <v>0</v>
@@ -2144,13 +2137,13 @@
         <v>2</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="S8" s="9" t="s">
         <v>80</v>
@@ -2164,16 +2157,16 @@
         <v>2</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>140</v>
+        <v>13</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>60</v>
+        <v>181</v>
       </c>
       <c r="S9" s="9" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
@@ -2184,13 +2177,13 @@
         <v>0</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="S10" s="9" t="s">
         <v>25</v>
@@ -2208,7 +2201,7 @@
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="13" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="S11" s="9" t="s">
         <v>20</v>
@@ -2219,331 +2212,298 @@
         <v>7</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="S12" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>8</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>129</v>
+        <v>25</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>144</v>
+        <v>31</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>145</v>
+        <v>35</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="S13" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>9</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>129</v>
+        <v>25</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>146</v>
+        <v>52</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>150</v>
+        <v>72</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="S14" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>10</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" customFormat="1" ht="67.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:19" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="33" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="33" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="9">
+        <v>1</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="S20" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="9">
+        <v>2</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E21" s="35"/>
+      <c r="S21" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="9">
+        <v>3</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="E22" s="35"/>
+      <c r="S22" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="S15" s="9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="9">
+    </row>
+    <row r="23" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="9">
+        <v>4</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E23" s="35"/>
+      <c r="S23" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="9">
+        <v>5</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E24" s="35"/>
+      <c r="S24" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="9">
+        <v>6</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E25" s="36"/>
+    </row>
+    <row r="26" spans="1:19" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="9">
+        <v>7</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="9">
+        <v>8</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E27" s="32"/>
+    </row>
+    <row r="28" spans="1:19" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="9">
+        <v>9</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E28" s="32"/>
+    </row>
+    <row r="29" spans="1:19" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="9">
+        <v>10</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="9">
         <v>11</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="S16" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9">
-        <v>12</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="S17" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="9">
-        <v>13</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C18" s="7" t="s">
+      <c r="B30" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9">
-        <v>14</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9">
-        <v>15</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="E20" s="30"/>
-    </row>
-    <row r="21" spans="1:19" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="9">
-        <v>16</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="E21" s="30"/>
-    </row>
-    <row r="22" spans="1:19" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="9">
-        <v>17</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="9">
-        <v>18</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" s="7" t="s">
+    </row>
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="2:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="2:5" ht="119.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="32" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="9">
-        <v>19</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="9">
-        <v>20</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="9">
-        <v>21</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="9">
-        <v>22</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="9">
-        <v>23</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:19" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="2:5" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="33"/>
-      <c r="C34"/>
-      <c r="D34"/>
-      <c r="E34"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="S1:S19">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="S1:S26">
     <sortCondition ref="S1"/>
   </sortState>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="E20:E25"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B30" xr:uid="{00000000-0002-0000-0200-000000000000}">
-      <formula1>$S$1:$S$21</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B15 B20:B32" xr:uid="{00000000-0002-0000-0200-000000000000}">
+      <formula1>$S$1:$S$28</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Seferler: dialog tabanlı planlama ve UI güncellemeleri
</commit_message>
<xml_diff>
--- a/DEV_NOTES/isleyis_semalari.xlsx
+++ b/DEV_NOTES/isleyis_semalari.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asil\SATTUP\DEV_NOTES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayhan\SATTUP\DEV_NOTES\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA5E67F-E14D-4D20-A01C-3B478E7D957C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sözleşmeler" sheetId="4" r:id="rId1"/>
@@ -577,7 +578,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -767,59 +768,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1109,35 +1110,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F46"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="93.7109375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" style="9" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="13.88671875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="93.6640625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" style="9" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1150,20 +1151,20 @@
       <c r="D5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="F5" s="18"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="23"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="22"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
       <c r="E6" s="14" t="s">
         <v>117</v>
       </c>
@@ -1171,7 +1172,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>0</v>
       </c>
@@ -1191,7 +1192,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>2</v>
       </c>
@@ -1207,7 +1208,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>0</v>
       </c>
@@ -1227,7 +1228,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>2</v>
       </c>
@@ -1247,7 +1248,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>2</v>
       </c>
@@ -1267,7 +1268,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>2</v>
       </c>
@@ -1287,7 +1288,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -1307,7 +1308,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>16</v>
       </c>
@@ -1327,7 +1328,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>20</v>
       </c>
@@ -1337,17 +1338,17 @@
       <c r="C15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="24" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>20</v>
       </c>
@@ -1357,11 +1358,11 @@
       <c r="C16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D16" s="26"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>2</v>
       </c>
@@ -1377,7 +1378,7 @@
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>2</v>
       </c>
@@ -1393,7 +1394,7 @@
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>2</v>
       </c>
@@ -1409,7 +1410,7 @@
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>25</v>
       </c>
@@ -1425,7 +1426,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>25</v>
       </c>
@@ -1441,7 +1442,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>25</v>
       </c>
@@ -1457,7 +1458,7 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>25</v>
       </c>
@@ -1473,7 +1474,7 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>39</v>
       </c>
@@ -1487,17 +1488,17 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>3</v>
       </c>
@@ -1511,17 +1512,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>47</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="21"/>
-      <c r="D30" s="22"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>39</v>
       </c>
@@ -1533,7 +1534,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>25</v>
       </c>
@@ -1547,7 +1548,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>25</v>
       </c>
@@ -1561,7 +1562,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>25</v>
       </c>
@@ -1575,7 +1576,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>25</v>
       </c>
@@ -1589,30 +1590,30 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="18" t="s">
         <v>58</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="25" t="s">
+      <c r="C37" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="D37" s="25"/>
-    </row>
-    <row r="38" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="24"/>
+      <c r="D37" s="19"/>
+    </row>
+    <row r="38" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="18"/>
       <c r="B38" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="26" t="s">
+      <c r="C38" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="D38" s="27"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
+      <c r="D38" s="21"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="18"/>
       <c r="B39" s="7" t="s">
         <v>67</v>
       </c>
@@ -1621,8 +1622,8 @@
       </c>
       <c r="D39" s="7"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="24"/>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="18"/>
       <c r="B40" s="7" t="s">
         <v>10</v>
       </c>
@@ -1631,8 +1632,8 @@
       </c>
       <c r="D40" s="7"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="24"/>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="18"/>
       <c r="B41" s="7" t="s">
         <v>11</v>
       </c>
@@ -1641,8 +1642,8 @@
       </c>
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="24"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="18"/>
       <c r="B42" s="7" t="s">
         <v>12</v>
       </c>
@@ -1651,8 +1652,8 @@
       </c>
       <c r="D42" s="7"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="18"/>
       <c r="B43" s="7" t="s">
         <v>40</v>
       </c>
@@ -1661,8 +1662,8 @@
       </c>
       <c r="D43" s="7"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="24"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="18"/>
       <c r="B44" s="7" t="s">
         <v>49</v>
       </c>
@@ -1671,71 +1672,71 @@
       </c>
       <c r="D44" s="7"/>
     </row>
-    <row r="45" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="24"/>
+    <row r="45" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="18"/>
       <c r="B45" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C45" s="26" t="s">
+      <c r="C45" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="D45" s="27"/>
-    </row>
-    <row r="46" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="24"/>
+      <c r="D45" s="21"/>
+    </row>
+    <row r="46" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="18"/>
       <c r="B46" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="26" t="s">
+      <c r="C46" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="D46" s="27"/>
+      <c r="D46" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="D15:D16"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="A37:A46"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="D15:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:D31"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="91.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="91.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1749,17 +1750,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="29"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1773,7 +1774,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>80</v>
       </c>
@@ -1787,7 +1788,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
@@ -1801,7 +1802,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>39</v>
       </c>
@@ -1813,7 +1814,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -1827,7 +1828,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
@@ -1841,19 +1842,19 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>3</v>
       </c>
@@ -1867,17 +1868,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="29"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="27"/>
+      <c r="D18" s="28"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>88</v>
       </c>
@@ -1891,7 +1892,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>88</v>
       </c>
@@ -1905,7 +1906,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -1919,13 +1920,13 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1939,7 +1940,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>25</v>
       </c>
@@ -1953,20 +1954,20 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>58</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="30" t="s">
+      <c r="C26" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="30"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="29"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="1" t="s">
         <v>67</v>
@@ -1976,7 +1977,7 @@
       </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="1" t="s">
         <v>81</v>
@@ -1986,7 +1987,7 @@
       </c>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="1" t="s">
         <v>83</v>
@@ -1996,7 +1997,7 @@
       </c>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="1" t="s">
         <v>12</v>
@@ -2006,7 +2007,7 @@
       </c>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="1" t="s">
         <v>85</v>
@@ -2027,31 +2028,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="91.140625" style="9" customWidth="1"/>
-    <col min="6" max="18" width="8.85546875" style="9"/>
-    <col min="19" max="19" width="18.42578125" style="9" customWidth="1"/>
-    <col min="20" max="16384" width="8.85546875" style="9"/>
+    <col min="1" max="1" width="5.5546875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="91.109375" style="9" customWidth="1"/>
+    <col min="6" max="18" width="8.88671875" style="9"/>
+    <col min="19" max="19" width="18.44140625" style="9" customWidth="1"/>
+    <col min="20" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="S1" s="9" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
         <v>130</v>
       </c>
@@ -2059,7 +2060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
         <v>131</v>
       </c>
@@ -2067,12 +2068,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="S4" s="9" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>143</v>
       </c>
@@ -2092,7 +2093,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>1</v>
       </c>
@@ -2102,13 +2103,13 @@
       <c r="C6" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="32"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="31"/>
       <c r="S6" s="9" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>2</v>
       </c>
@@ -2128,7 +2129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>3</v>
       </c>
@@ -2148,7 +2149,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>4</v>
       </c>
@@ -2168,7 +2169,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>5</v>
       </c>
@@ -2188,7 +2189,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>6</v>
       </c>
@@ -2206,7 +2207,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>7</v>
       </c>
@@ -2221,7 +2222,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>8</v>
       </c>
@@ -2238,7 +2239,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>9</v>
       </c>
@@ -2255,7 +2256,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>10</v>
       </c>
@@ -2272,19 +2273,19 @@
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:19" customFormat="1" ht="67.900000000000006" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:19" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
+    <row r="16" spans="1:19" customFormat="1" ht="67.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:19" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="33" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="1:19" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="16" t="s">
+    <row r="18" spans="1:19" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="33" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <v>1</v>
       </c>
@@ -2304,7 +2305,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
         <v>2</v>
       </c>
@@ -2322,7 +2323,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
         <v>3</v>
       </c>
@@ -2340,7 +2341,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9">
         <v>4</v>
       </c>
@@ -2358,7 +2359,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
         <v>5</v>
       </c>
@@ -2376,7 +2377,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9">
         <v>6</v>
       </c>
@@ -2391,7 +2392,7 @@
       </c>
       <c r="E25" s="36"/>
     </row>
-    <row r="26" spans="1:19" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9">
         <v>7</v>
       </c>
@@ -2404,11 +2405,11 @@
       <c r="D26" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="E26" s="33" t="s">
+      <c r="E26" s="32" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
         <v>8</v>
       </c>
@@ -2421,9 +2422,9 @@
       <c r="D27" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E27" s="33"/>
-    </row>
-    <row r="28" spans="1:19" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="32"/>
+    </row>
+    <row r="28" spans="1:19" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9">
         <v>9</v>
       </c>
@@ -2436,9 +2437,9 @@
       <c r="D28" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E28" s="33"/>
-    </row>
-    <row r="29" spans="1:19" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="32"/>
+    </row>
+    <row r="29" spans="1:19" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9">
         <v>10</v>
       </c>
@@ -2455,7 +2456,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9">
         <v>11</v>
       </c>
@@ -2472,26 +2473,26 @@
         <v>176</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="2:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="2:5" ht="119.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="2:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="2:5" ht="119.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="33" t="s">
+      <c r="C35" s="32" t="s">
         <v>177</v>
       </c>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C36"/>
       <c r="D36"/>
       <c r="E36"/>
     </row>
   </sheetData>
-  <sortState ref="S1:S26">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="S1:S26">
     <sortCondition ref="S1"/>
   </sortState>
   <mergeCells count="4">
@@ -2501,7 +2502,7 @@
     <mergeCell ref="E20:E25"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B15 B20:B32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B15 B20:B32" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>$S$1:$S$28</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>